<commit_message>
atualizar os exercicios feitos em CSS Avançado - parte 2
</commit_message>
<xml_diff>
--- a/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
+++ b/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
@@ -1288,9 +1288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>70920</xdr:colOff>
+      <xdr:colOff>70560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1304,7 +1304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="423000" y="133200"/>
-          <a:ext cx="961200" cy="180360"/>
+          <a:ext cx="960840" cy="180000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2042,8 +2042,8 @@
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
-      <c r="B31" s="17" t="s">
-        <v>20</v>
+      <c r="B31" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>34</v>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="C61" s="20" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B61)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="C62" s="22" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B62)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Exercicios feitos de SNA
</commit_message>
<xml_diff>
--- a/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
+++ b/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <r>
       <rPr>
@@ -609,109 +609,112 @@
     <t xml:space="preserve">ETAPA 2 - DO DIA 16/03/2024 AO DIA 29/03/2024</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GIT/GITHUB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - FLEXBOX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "GIT/GITHUB"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/Git-Programa-de-versionamento-000aef645b5c452d87a7fe366d132498?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CLEAN CODE"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/Clean-Code-a1dd6982d21e45c98959f1aa14cd4252?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 INTERMEDIÁRIO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/HTML-Intermedi-rio-d2e0d5f5fdda47ceba89b0767f8383fa?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS INTERMEDIÁRIO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Intermedi-rio-85df267a276e4543bd7bcdc0a18f12ed?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 AVANÇADO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/HTML-Avan-ado-0179b3307db54ad1a600779b55742427?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte1-35278f1d44314a23b6317d7dccf6b020?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 2 - FLEXBOX"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte-2-b6a0869bbc66489083cbd184d9c2200a?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - FLEXBOX"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/mfdzerohour/DevEmDobro/tree/main/DeVEmDobro_Curso/008_-_%20Exerc%C3%ADcios_CSS_avan%C3%A7ado_-_Flexbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 3 - DO DIA 30/03/2024 AO DIA 12/04/2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">PENDENTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GIT/GITHUB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - FLEXBOX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "GIT/GITHUB"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/Git-Programa-de-versionamento-000aef645b5c452d87a7fe366d132498?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CLEAN CODE"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/Clean-Code-a1dd6982d21e45c98959f1aa14cd4252?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 INTERMEDIÁRIO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/HTML-Intermedi-rio-d2e0d5f5fdda47ceba89b0767f8383fa?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS INTERMEDIÁRIO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Intermedi-rio-85df267a276e4543bd7bcdc0a18f12ed?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 AVANÇADO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/HTML-Avan-ado-0179b3307db54ad1a600779b55742427?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte1-35278f1d44314a23b6317d7dccf6b020?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 2 - FLEXBOX"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte-2-b6a0869bbc66489083cbd184d9c2200a?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - FLEXBOX"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 3 - DO DIA 30/03/2024 AO DIA 12/04/2024</t>
   </si>
   <si>
     <r>
@@ -1288,9 +1291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>70560</xdr:colOff>
+      <xdr:colOff>70200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1304,7 +1307,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="423000" y="133200"/>
-          <a:ext cx="960840" cy="180000"/>
+          <a:ext cx="960480" cy="179640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1498,8 +1501,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1897,11 +1900,11 @@
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -1920,14 +1923,14 @@
         <v>8</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1941,14 +1944,14 @@
         <v>8</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -1962,14 +1965,14 @@
         <v>8</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -1983,14 +1986,14 @@
         <v>8</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -2004,14 +2007,14 @@
         <v>8</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -2025,14 +2028,14 @@
         <v>8</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -2046,14 +2049,14 @@
         <v>8</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -2063,17 +2066,19 @@
     </row>
     <row r="32" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
-      <c r="B32" s="17" t="s">
-        <v>20</v>
+      <c r="B32" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
@@ -2150,10 +2155,10 @@
     <row r="38" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -2169,10 +2174,10 @@
     <row r="39" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -2206,7 +2211,7 @@
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -2255,10 +2260,10 @@
     <row r="45" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
@@ -2274,10 +2279,10 @@
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
@@ -2293,10 +2298,10 @@
     <row r="47" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -2312,10 +2317,10 @@
     <row r="48" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
@@ -2349,7 +2354,7 @@
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -2398,10 +2403,10 @@
     <row r="54" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -2417,10 +2422,10 @@
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="17" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
@@ -2483,11 +2488,11 @@
     </row>
     <row r="61" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="19" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C61" s="20" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B61)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2496,7 +2501,7 @@
       </c>
       <c r="C62" s="22" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B62)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Atualização da Planilha meu primeiro site
</commit_message>
<xml_diff>
--- a/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
+++ b/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
@@ -714,133 +714,133 @@
     <t xml:space="preserve">ETAPA 3 - DO DIA 30/03/2024 AO DIA 12/04/2024</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CSS AVANÇADO parte 3 - GRID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - GRID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - GRID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 4 - DO DIA 13/04/2024 AO DIA 26/04/2024</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CSS MÓDULO DE REFORÇO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"QUEST HTML E CSS AVANÇADO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS MÓDULO DE REFORÇO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "PROJETO LP COM FLEX E GRID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEST "HTML E CSS AVANÇADO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 5 - DO DIA 27/04/2024 AO DIA 10/05/2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">PENDENTE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSS AVANÇADO parte 3 - GRID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - GRID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - GRID"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 4 - DO DIA 13/04/2024 AO DIA 26/04/2024</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSS MÓDULO DE REFORÇO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"QUEST HTML E CSS AVANÇADO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS MÓDULO DE REFORÇO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "PROJETO LP COM FLEX E GRID"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUEST "HTML E CSS AVANÇADO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 5 - DO DIA 27/04/2024 AO DIA 10/05/2024</t>
   </si>
   <si>
     <r>
@@ -1291,9 +1291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>70200</xdr:colOff>
+      <xdr:colOff>69840</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>179640</xdr:rowOff>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1307,7 +1307,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="423000" y="133200"/>
-          <a:ext cx="960480" cy="179640"/>
+          <a:ext cx="960120" cy="179280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1501,8 +1501,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2154,11 +2154,11 @@
     </row>
     <row r="38" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -2173,11 +2173,11 @@
     </row>
     <row r="39" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
-      <c r="B39" s="17" t="s">
-        <v>38</v>
+      <c r="B39" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -2211,7 +2211,7 @@
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -2259,11 +2259,11 @@
     </row>
     <row r="45" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
-      <c r="B45" s="17" t="s">
-        <v>38</v>
+      <c r="B45" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
@@ -2278,11 +2278,11 @@
     </row>
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
-      <c r="B46" s="17" t="s">
-        <v>38</v>
+      <c r="B46" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
@@ -2297,11 +2297,11 @@
     </row>
     <row r="47" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
-      <c r="B47" s="17" t="s">
-        <v>38</v>
+      <c r="B47" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -2316,11 +2316,11 @@
     </row>
     <row r="48" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
-      <c r="B48" s="17" t="s">
-        <v>38</v>
+      <c r="B48" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
@@ -2354,7 +2354,7 @@
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
@@ -2403,7 +2403,7 @@
     <row r="54" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="17" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>47</v>
@@ -2422,7 +2422,7 @@
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="17" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>48</v>
@@ -2488,11 +2488,11 @@
     </row>
     <row r="61" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="19" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C61" s="20" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B61)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="C62" s="22" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B62)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Criando o portfolio inicial do sistema
</commit_message>
<xml_diff>
--- a/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
+++ b/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
@@ -1507,8 +1507,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2412,8 +2412,8 @@
     </row>
     <row r="54" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
-      <c r="B54" s="14" t="s">
-        <v>18</v>
+      <c r="B54" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>49</v>
@@ -2502,7 +2502,7 @@
       </c>
       <c r="C61" s="20" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B61)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="C62" s="22" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B62)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Todos os desafios completos
</commit_message>
<xml_diff>
--- a/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
+++ b/9999 - Desafios propostos/001 - SNA (Sistema de Navegação do Aluno) e MPS (Meu Primeiro Site).xlsx
@@ -603,276 +603,276 @@
     <t xml:space="preserve">https://www.notion.so/CSS-B-sico-75b9a40005fb435d923137c8a8ff0234?pvs=4</t>
   </si>
   <si>
+    <t xml:space="preserve">EXERCÍCIOS "HTML E CSS BÁSICO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 2 - DO DIA 16/03/2024 AO DIA 29/03/2024</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GIT/GITHUB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - FLEXBOX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "GIT/GITHUB"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/Git-Programa-de-versionamento-000aef645b5c452d87a7fe366d132498?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CLEAN CODE"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/Clean-Code-a1dd6982d21e45c98959f1aa14cd4252?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 INTERMEDIÁRIO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/HTML-Intermedi-rio-d2e0d5f5fdda47ceba89b0767f8383fa?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS INTERMEDIÁRIO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Intermedi-rio-85df267a276e4543bd7bcdc0a18f12ed?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 AVANÇADO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/HTML-Avan-ado-0179b3307db54ad1a600779b55742427?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte1-35278f1d44314a23b6317d7dccf6b020?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 2 - FLEXBOX"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte-2-b6a0869bbc66489083cbd184d9c2200a?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - FLEXBOX"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/mfdzerohour/DevEmDobro/tree/main/DeVEmDobro_Curso/008_-_%20Exerc%C3%ADcios_CSS_avan%C3%A7ado_-_Flexbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 3 - DO DIA 30/03/2024 AO DIA 12/04/2024</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CSS AVANÇADO parte 3 - GRID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - GRID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - GRID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 4 - DO DIA 13/04/2024 AO DIA 26/04/2024</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CSS MÓDULO DE REFORÇO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">" ATÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"QUEST HTML E CSS AVANÇADO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "CSS MÓDULO DE REFORÇO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/CSS-Refor-o-Criar-uma-p-gina-sem-Travar-1-ca3e75b0ad464480a2565c860cf70044?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESUMO DO MÓDULO "PROJETO LP COM FLEX E GRID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.notion.so/Projeto-Land-Page-Flexbox-e-Grid-caa3823176b94be5a6538e0f3a684018?pvs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEST "HTML E CSS AVANÇADO"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETAPA 5 - DO DIA 27/04/2024 AO DIA 10/05/2024</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COMPLETAR AS AULAS DO MÓDULO BÔNUS </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"DEEP DIVES - CRIANDO UM PORTFÓLIO F#D#"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">⭐SEU PORTFÓLIO PERSONALIZADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">PENDENTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXERCÍCIOS "HTML E CSS BÁSICO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 2 - DO DIA 16/03/2024 AO DIA 29/03/2024</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GIT/GITHUB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - FLEXBOX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "GIT/GITHUB"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/Git-Programa-de-versionamento-000aef645b5c452d87a7fe366d132498?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CLEAN CODE"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/Clean-Code-a1dd6982d21e45c98959f1aa14cd4252?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 INTERMEDIÁRIO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/HTML-Intermedi-rio-d2e0d5f5fdda47ceba89b0767f8383fa?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS INTERMEDIÁRIO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Intermedi-rio-85df267a276e4543bd7bcdc0a18f12ed?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "HTML 5 AVANÇADO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/HTML-Avan-ado-0179b3307db54ad1a600779b55742427?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte1-35278f1d44314a23b6317d7dccf6b020?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS AVANÇADO parte 2 - FLEXBOX"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Avan-ado-parte-2-b6a0869bbc66489083cbd184d9c2200a?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - FLEXBOX"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/mfdzerohour/DevEmDobro/tree/main/DeVEmDobro_Curso/008_-_%20Exerc%C3%ADcios_CSS_avan%C3%A7ado_-_Flexbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 3 - DO DIA 30/03/2024 AO DIA 12/04/2024</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSS AVANÇADO parte 3 - GRID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"EXERCÍCIOS CSS AVANÇADO - GRID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">EXERCÍCIOS "CSS AVANÇADO - GRID"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 4 - DO DIA 13/04/2024 AO DIA 26/04/2024</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DOS MÓDULOS "</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">CSS MÓDULO DE REFORÇO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">" ATÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"QUEST HTML E CSS AVANÇADO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "CSS MÓDULO DE REFORÇO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/CSS-Refor-o-Criar-uma-p-gina-sem-Travar-1-ca3e75b0ad464480a2565c860cf70044?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUMO DO MÓDULO "PROJETO LP COM FLEX E GRID"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.notion.so/Projeto-Land-Page-Flexbox-e-Grid-caa3823176b94be5a6538e0f3a684018?pvs=4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUEST "HTML E CSS AVANÇADO"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETAPA 5 - DO DIA 27/04/2024 AO DIA 10/05/2024</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COMPLETAR AS AULAS DO MÓDULO BÔNUS </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"DEEP DIVES - CRIANDO UM PORTFÓLIO F#D#"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">⭐SEU PORTFÓLIO PERSONALIZADO</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1155,7 +1155,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1171,10 +1171,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1199,7 +1195,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1207,7 +1203,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1297,9 +1293,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>69480</xdr:colOff>
+      <xdr:colOff>69120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:rowOff>178560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1313,7 +1309,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="423000" y="133200"/>
-          <a:ext cx="959760" cy="178920"/>
+          <a:ext cx="959400" cy="178560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1507,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1820,59 +1816,59 @@
     </row>
     <row r="18" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
-      <c r="B21" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1910,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -1929,14 +1925,14 @@
         <v>8</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1950,14 +1946,14 @@
         <v>8</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -1971,20 +1967,20 @@
         <v>8</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
+      <c r="H27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
@@ -1992,20 +1988,20 @@
         <v>8</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
+      <c r="H28" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
@@ -2013,20 +2009,20 @@
         <v>8</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
+      <c r="H29" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
@@ -2034,20 +2030,20 @@
         <v>8</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
+      <c r="H30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
@@ -2055,20 +2051,20 @@
         <v>8</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
+      <c r="H31" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
@@ -2076,57 +2072,57 @@
         <v>8</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
+      <c r="H32" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
-      <c r="B35" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2164,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -2183,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -2199,39 +2195,39 @@
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
-      <c r="B42" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2269,7 +2265,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
@@ -2288,14 +2284,14 @@
         <v>8</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
@@ -2309,14 +2305,14 @@
         <v>8</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -2326,57 +2322,57 @@
     </row>
     <row r="48" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
-      <c r="B48" s="14" t="s">
-        <v>18</v>
+      <c r="B48" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
-      <c r="B51" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
+      <c r="B51" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
@@ -2416,7 +2412,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -2431,16 +2427,16 @@
     </row>
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
-      <c r="B55" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="B55" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
@@ -2497,25 +2493,25 @@
       <c r="M59" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" s="20" t="n">
+      <c r="B61" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" s="19" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B61)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="22" t="n">
+      <c r="C62" s="21" t="n">
         <f aca="false">COUNTIF($B$13:$B$56,B62)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="23"/>
+      <c r="C63" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="72">

</xml_diff>